<commit_message>
Menus, Updated Icons, Documentation
In progress changes to menus, I simplified the food icons, and added a bit of styling. Also updated the project documentation.
</commit_message>
<xml_diff>
--- a/files/menus/arrowsmith_grill/breakfast_arrowsmith.xlsx
+++ b/files/menus/arrowsmith_grill/breakfast_arrowsmith.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ollip\Documents\!!ProjectFiles\ezrab_feedbc\files\menus\arrowsmith_grill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E13F0AB-AFF6-4270-9B71-AC806946E6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1B9E5B-DA6C-4889-8169-173E033B68D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="3510" windowWidth="24825" windowHeight="14220" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
+    <workbookView xWindow="7665" yWindow="2490" windowWidth="27915" windowHeight="15705" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Ingredients</t>
   </si>
@@ -53,9 +53,6 @@
     <t>nutritionLabel</t>
   </si>
   <si>
-    <t>waffles</t>
-  </si>
-  <si>
     <t>Egg, Sausage</t>
   </si>
   <si>
@@ -93,13 +90,73 @@
   </si>
   <si>
     <t>Veggie Breakfast Burrito</t>
+  </si>
+  <si>
+    <t>Sausage Breakfast Sandwich</t>
+  </si>
+  <si>
+    <t>Muffin / Cooked Sausage Round / Cooked Egg Round / Pasteurized Process Cheddar Cheese</t>
+  </si>
+  <si>
+    <t>Soy, wheat, milk, eggs.</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Sausage_Breakfast_Sandwich</t>
+  </si>
+  <si>
+    <t>Bacon Breakfast Sandwich</t>
+  </si>
+  <si>
+    <t>English Muffin / Egg Patty / Processed Cheddar Cheese / Bacon.</t>
+  </si>
+  <si>
+    <t>Bacon_Breakfast_Sandwich</t>
+  </si>
+  <si>
+    <t>Egg and Cheese Breakfast Sandwich</t>
+  </si>
+  <si>
+    <t>English Muffin / Egg Patty / Processed Cheddar Cheese</t>
+  </si>
+  <si>
+    <t>VEG</t>
+  </si>
+  <si>
+    <t>Egg_and_Cheese_Breakfast_Sandwich</t>
+  </si>
+  <si>
+    <t>VGN</t>
+  </si>
+  <si>
+    <t>placeholder</t>
+  </si>
+  <si>
+    <t>Breakfast Waffles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgian-style Waffles / Whipped Cream / Seasonal Fruit Compote or Maple Syrup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wheat, milk, eggs, </t>
+  </si>
+  <si>
+    <t>Beef Sausage Roll</t>
+  </si>
+  <si>
+    <t>Tofu Scramble Roll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spicy Chicken Sausage Roll </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,16 +170,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FFC6E0B4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,15 +200,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,8 +246,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}" name="Table3" displayName="Table3" ref="A1:G4" totalsRowShown="0">
-  <autoFilter ref="A1:G4" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}" name="Table3" displayName="Table3" ref="A1:G11" totalsRowShown="0">
+  <autoFilter ref="A1:G11" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AA44CCDF-F9E2-4FB6-9AED-85FE3A3C6008}" name="ItemName"/>
     <tableColumn id="2" xr3:uid="{9D7FC130-DF66-4465-8F0B-6015043C6AA1}" name="Ingredients"/>
@@ -469,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E4FEC9-4E15-443B-89A8-5C76E19963E8}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -505,67 +594,175 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleared empty cells and replaced all  unfinished items with placeholders
</commit_message>
<xml_diff>
--- a/files/menus/arrowsmith_grill/breakfast_arrowsmith.xlsx
+++ b/files/menus/arrowsmith_grill/breakfast_arrowsmith.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ollip\Documents\!!ProjectFiles\ezrab_feedbc\files\menus\arrowsmith_grill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0690B58C-FE57-4116-B3B9-DFD2F36D3A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52ADD45-3826-4920-AE37-3204C3F02E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="8250" windowWidth="27915" windowHeight="15705" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
+    <workbookView xWindow="9975" yWindow="1860" windowWidth="27915" windowHeight="15705" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
   </bookViews>
   <sheets>
     <sheet name="breakfast_arrowsmith" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Ingredients</t>
   </si>
@@ -579,7 +579,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,10 +785,15 @@
       <c r="C10" t="s">
         <v>42</v>
       </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Added Nutri Labels. Changed Layouts.
Altered view heights  and completed all nutritional breakdowns.
</commit_message>
<xml_diff>
--- a/files/menus/arrowsmith_grill/breakfast_arrowsmith.xlsx
+++ b/files/menus/arrowsmith_grill/breakfast_arrowsmith.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ollip\Documents\!!ProjectFiles\ezrab_feedbc\files\menus\arrowsmith_grill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52ADD45-3826-4920-AE37-3204C3F02E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACC2A93-C0D8-4213-A64E-00658CEA62A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9975" yWindow="1860" windowWidth="27915" windowHeight="15705" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
+    <workbookView xWindow="17565" yWindow="2850" windowWidth="21285" windowHeight="13215" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
   </bookViews>
   <sheets>
     <sheet name="breakfast_arrowsmith" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Ingredients</t>
   </si>
@@ -53,27 +53,9 @@
     <t>nutritionLabel</t>
   </si>
   <si>
-    <t>Egg, Sausage</t>
-  </si>
-  <si>
-    <t>Potato</t>
-  </si>
-  <si>
-    <t>Turkey / Bacon / Cheddar Cheese / Lettuce / Tomato / Garlic Aioli</t>
-  </si>
-  <si>
-    <t>Turkey / Swiss Cheese / Roasted Onion / Tomato / Cucumber / Mixed Greens / Spicy Mayo</t>
-  </si>
-  <si>
-    <t>Falafel / Feta / Red Onion / Cucumber / Mixed Greens / Tomato / Tzatziki</t>
-  </si>
-  <si>
     <t>Allergens</t>
   </si>
   <si>
-    <t>Wheat, sulphites, egg.</t>
-  </si>
-  <si>
     <t>LeaveEmpty</t>
   </si>
   <si>
@@ -128,12 +110,6 @@
     <t>Egg_and_Cheese_Breakfast_Sandwich</t>
   </si>
   <si>
-    <t>VGN</t>
-  </si>
-  <si>
-    <t>placeholder</t>
-  </si>
-  <si>
     <t>Breakfast Waffles</t>
   </si>
   <si>
@@ -155,19 +131,58 @@
     <t>Wheat, soy.</t>
   </si>
   <si>
-    <t>pastry / tofu / seasonings</t>
-  </si>
-  <si>
-    <t>pastry / beef / seasonings</t>
-  </si>
-  <si>
-    <t>pastry / chicken sausage / seasonings</t>
-  </si>
-  <si>
-    <t>Wheat, milk, eggs, soy.</t>
-  </si>
-  <si>
     <t>Patisserie LeBeau Waffles</t>
+  </si>
+  <si>
+    <t>BC,VEG</t>
+  </si>
+  <si>
+    <t>Eggs / Bacon / Tater Tots /  Salsa / Nacho Cheese</t>
+  </si>
+  <si>
+    <t>Wheat, milk, sulphites, egg.</t>
+  </si>
+  <si>
+    <t>Castle Cheese Nacho Blend</t>
+  </si>
+  <si>
+    <t>Eggs / Pork Sausage / Tater Tots /  Salsa / Nacho Cheese</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Castle Cheese Nacho Blend</t>
+  </si>
+  <si>
+    <t>Eggs / Spinach / Tater Tots /  Salsa / Nacho Cheese</t>
+  </si>
+  <si>
+    <t>BC,VGN,DF</t>
+  </si>
+  <si>
+    <t>Maureen's Tofu Roll</t>
+  </si>
+  <si>
+    <t>Flaky Pastry / Ground Beef Sausage / Spices</t>
+  </si>
+  <si>
+    <t>Flaky Pastry / Ground Seasoned Chicken Sausage / Spices</t>
+  </si>
+  <si>
+    <t>Flaky Pastry / Tofu Scramble / Spices</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>Tofu_Scramble_Roll</t>
+  </si>
+  <si>
+    <t>Beef_Sausage_Roll</t>
+  </si>
+  <si>
+    <t>Bacon_Breakfast_Burrito</t>
+  </si>
+  <si>
+    <t>Falafel_Wrap</t>
   </si>
 </sst>
 </file>
@@ -579,7 +594,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -612,207 +627,207 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>31</v>
+      <c r="F11" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>